<commit_message>
Poprawiony schemat oraz wartości komponentów
</commit_message>
<xml_diff>
--- a/dokumentacja.xlsx
+++ b/dokumentacja.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piotr\Documents\mos\laser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F3EB0A-3A5D-413D-BBF3-59D0DF152E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8278BD97-1D21-4F41-8369-ABFCE178569D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" activeTab="1" xr2:uid="{C786B773-E517-459C-88A4-5CBE983CE902}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C786B773-E517-459C-88A4-5CBE983CE902}"/>
   </bookViews>
   <sheets>
     <sheet name="Wartości" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
   <si>
     <t>Nazwa</t>
   </si>
@@ -359,9 +359,6 @@
     <t>Wybrana wartość</t>
   </si>
   <si>
-    <t>współczynnik tętnienia (limit 30% tętnienia)</t>
-  </si>
-  <si>
     <r>
       <t>R</t>
     </r>
@@ -594,9 +591,6 @@
     </r>
   </si>
   <si>
-    <t>pojemność kondensatora wyjściowego</t>
-  </si>
-  <si>
     <t>minimalna impedancja na kondensatorze wyjściowym</t>
   </si>
   <si>
@@ -1376,6 +1370,15 @@
   </si>
   <si>
     <t xml:space="preserve">    Z obliczeń (zmieniać na drugiej stronie):</t>
+  </si>
+  <si>
+    <t>µH</t>
+  </si>
+  <si>
+    <t>współczynnik tętnienia (limit 20% tętnienia)</t>
+  </si>
+  <si>
+    <t>pojemność kondensatora wyjściowego x2</t>
   </si>
 </sst>
 </file>
@@ -1552,6 +1555,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1561,8 +1566,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2174,18 +2177,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62F3686-4B1B-47EE-BF8D-2E96173711F6}">
   <dimension ref="B2:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.350000000000001" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.21875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="5.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47" style="1" customWidth="1"/>
     <col min="7" max="8" width="8.88671875" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.77734375" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" style="1"/>
@@ -2217,7 +2220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
@@ -2232,7 +2235,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>34</v>
       </c>
@@ -2247,7 +2250,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
@@ -2262,7 +2265,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>36</v>
       </c>
@@ -2277,9 +2280,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="20.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="3">
         <v>0.4</v>
@@ -2289,10 +2292,10 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
         <v>37</v>
       </c>
@@ -2307,9 +2310,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="3">
         <v>0.02</v>
@@ -2322,22 +2325,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="5">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C13" s="3">
         <v>2.2000000000000002</v>
@@ -2347,12 +2350,12 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B14" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C14" s="3">
         <v>5</v>
@@ -2362,12 +2365,12 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -2382,9 +2385,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B16" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C16" s="5">
         <v>100</v>
@@ -2397,9 +2400,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -2414,9 +2417,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" s="5">
         <v>100</v>
@@ -2429,9 +2432,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -2446,12 +2449,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C20" s="5">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>30</v>
@@ -2461,9 +2464,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C21" s="5">
         <v>47</v>
@@ -2472,15 +2475,15 @@
         <v>38</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C22" s="5">
         <v>22</v>
@@ -2489,15 +2492,15 @@
         <v>38</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B23" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C23" s="5">
         <v>0.1</v>
@@ -2506,15 +2509,15 @@
         <v>38</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" s="3">
         <v>0.1</v>
@@ -2523,15 +2526,15 @@
         <v>38</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B25" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C25" s="3">
         <v>10</v>
@@ -2541,28 +2544,28 @@
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26" s="18" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C28" s="3">
         <f>Obliczenia!E3</f>
@@ -2572,49 +2575,49 @@
         <v>20</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="7">
         <f>Obliczenia!E5</f>
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B30" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" s="3">
         <f>Obliczenia!E10</f>
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>38</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B31" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C31" s="3">
         <f>Obliczenia!E14</f>
@@ -2624,23 +2627,23 @@
         <v>30</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="20.95" x14ac:dyDescent="0.45">
+      <c r="F31" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B32" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C32" s="3">
         <f>Obliczenia!E15</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E32" s="3"/>
-      <c r="F32" s="18"/>
+      <c r="F32" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2656,11 +2659,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A622F7-F2B0-4B49-9EE8-34CDB52550BF}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14:G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.109375" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
@@ -2668,10 +2671,10 @@
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.6640625" customWidth="1"/>
-    <col min="7" max="7" width="36.44140625" customWidth="1"/>
+    <col min="7" max="7" width="49.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.350000000000001" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2680,7 +2683,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="18.350000000000001" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2701,10 +2704,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="42.55" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="17" t="s">
-        <v>44</v>
+      <c r="B3" s="19" t="s">
+        <v>43</v>
       </c>
       <c r="C3" s="7" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2720,12 +2723,12 @@
         <v>20</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="41.9" customHeight="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="41.85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
-      <c r="B4" s="18"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7">
         <f>Wartości!C8^2*Obliczenia!E3</f>
@@ -2735,180 +2738,180 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="42.55" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="7" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
       <c r="D5" s="9">
         <f>(Wartości!C7*(Wartości!C6-Wartości!C7))/(Wartości!C6*Wartości!C12*Wartości!C8*Wartości!C5*1000)</f>
-        <v>1.3132716049382716E-5</v>
+        <v>1.9699074074074069E-5</v>
       </c>
       <c r="E5" s="15">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="42.55" customHeight="1" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="7" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="D6" s="13">
         <f>(Wartości!C7*(Wartości!C6-Wartości!C7))/(Wartości!C6*Wartości!C5*1000*Obliczenia!E5/1000000)</f>
-        <v>0.47277777777777774</v>
+        <v>0.32234848484848488</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="42.55" customHeight="1" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="7" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="D7" s="13">
         <f>Wartości!C8+(Obliczenia!D6/2)</f>
-        <v>2.0363888888888888</v>
+        <v>1.9611742424242424</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="41.9" customHeight="1" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="41.85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="7" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="D8" s="13">
         <f>SQRT(Wartości!C8^2+(Obliczenia!D6^2/12))</f>
-        <v>1.8051666319013437</v>
+        <v>1.8024036854915928</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="42.55" customHeight="1" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" s="7" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
       <c r="D9" s="11">
         <f>(Wartości!C9*Wartości!C11)/(Obliczenia!D6-Wartości!C11)</f>
-        <v>1.7668711656441721E-2</v>
+        <v>2.6459533951390626E-2</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="42.55" customHeight="1" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" s="7" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="D10" s="7">
         <f>1/(2*3.1415*Wartości!C5*1000*Obliczenia!D9)</f>
-        <v>2.2519983376660113E-5</v>
+        <v>1.5038023478457984E-5</v>
       </c>
       <c r="E10" s="15">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>38</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="42.55" customHeight="1" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" s="7" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
       <c r="D11" s="12">
         <f>1/(2*3.1415*Wartości!C5*1000*Obliczenia!E10/1000000)</f>
-        <v>1.2057548266365709E-2</v>
+        <v>9.0431611997742814E-3</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="42.55" customHeight="1" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" s="7" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="D12" s="12">
         <f>(D11*D6)/(D11+Wartości!C9)</f>
-        <v>1.3834331876225415E-2</v>
+        <v>7.1265078786249486E-3</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="42.55" customHeight="1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C13" s="7" t="e" vm="10">
         <v>#VALUE!</v>
@@ -2920,16 +2923,16 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="42.55" customHeight="1" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="D14" s="7">
         <v>56</v>
@@ -2940,28 +2943,28 @@
       <c r="F14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="42.55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D15" s="7">
         <v>44</v>
       </c>
       <c r="E15" s="15">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="18"/>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
@@ -3026,33 +3029,33 @@
   <dimension ref="B2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.5546875" customWidth="1"/>
     <col min="2" max="2" width="22.5546875" customWidth="1"/>
     <col min="3" max="3" width="146.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="19" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="18.350000000000001" x14ac:dyDescent="0.35">
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="2:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="18.350000000000001" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" s="21" t="s">
         <v>4</v>
       </c>
@@ -3060,7 +3063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="18.350000000000001" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" ht="18" x14ac:dyDescent="0.35">
       <c r="B5" s="21"/>
       <c r="C5" s="3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Poprawki do schematu oraz dobór footprintów i BOM
</commit_message>
<xml_diff>
--- a/dokumentacja.xlsx
+++ b/dokumentacja.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piotr\Documents\mos\laser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8278BD97-1D21-4F41-8369-ABFCE178569D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241BEA0D-6BEA-49D8-B05A-13988747313B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C786B773-E517-459C-88A4-5CBE983CE902}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{C786B773-E517-459C-88A4-5CBE983CE902}"/>
   </bookViews>
   <sheets>
     <sheet name="Wartości" sheetId="1" r:id="rId1"/>
     <sheet name="Obliczenia" sheetId="3" r:id="rId2"/>
     <sheet name="Dokumentacja" sheetId="2" r:id="rId3"/>
+    <sheet name="BOM" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -150,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="139">
   <si>
     <t>Nazwa</t>
   </si>
@@ -1379,6 +1380,108 @@
   </si>
   <si>
     <t>pojemność kondensatora wyjściowego x2</t>
+  </si>
+  <si>
+    <t>wartość</t>
+  </si>
+  <si>
+    <t>ilość</t>
+  </si>
+  <si>
+    <t>jednostka</t>
+  </si>
+  <si>
+    <t>cena za sztukę</t>
+  </si>
+  <si>
+    <t>uF</t>
+  </si>
+  <si>
+    <t>opis</t>
+  </si>
+  <si>
+    <t>rezystor</t>
+  </si>
+  <si>
+    <t>rezystor (0.5 W) pomiarowy</t>
+  </si>
+  <si>
+    <t>dioda</t>
+  </si>
+  <si>
+    <t>SS34</t>
+  </si>
+  <si>
+    <t>cewka</t>
+  </si>
+  <si>
+    <t>uH</t>
+  </si>
+  <si>
+    <t>op-amp</t>
+  </si>
+  <si>
+    <t>MCP6001-OT</t>
+  </si>
+  <si>
+    <t>stabilizator</t>
+  </si>
+  <si>
+    <t>AMS1117</t>
+  </si>
+  <si>
+    <t>driver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">potencjometr </t>
+  </si>
+  <si>
+    <t>cena</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>uwagi</t>
+  </si>
+  <si>
+    <t>digikey</t>
+  </si>
+  <si>
+    <t>mouser</t>
+  </si>
+  <si>
+    <t>TME</t>
+  </si>
+  <si>
+    <t>na razie nie dostępny na mouser</t>
+  </si>
+  <si>
+    <t>ilość min</t>
+  </si>
+  <si>
+    <t>kondensator ceramiczny</t>
+  </si>
+  <si>
+    <t>kondensator elektrolityczny</t>
+  </si>
+  <si>
+    <t>kondensator ceramiczny X7R 25V</t>
+  </si>
+  <si>
+    <t>konektor power</t>
+  </si>
+  <si>
+    <t>konektor input</t>
+  </si>
+  <si>
+    <t>konektor laser</t>
+  </si>
+  <si>
+    <t>JST 3 pin</t>
+  </si>
+  <si>
+    <t>JST 2 pin</t>
   </si>
 </sst>
 </file>
@@ -1390,7 +1493,7 @@
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1437,8 +1540,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1448,6 +1560,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1517,10 +1641,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1557,6 +1682,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1569,8 +1698,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2177,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62F3686-4B1B-47EE-BF8D-2E96173711F6}">
   <dimension ref="B2:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2548,20 +2681,20 @@
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
     </row>
     <row r="28" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
@@ -2627,7 +2760,7 @@
         <v>30</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="23" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2643,7 +2776,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="3"/>
-      <c r="F32" s="20"/>
+      <c r="F32" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2659,7 +2792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A622F7-F2B0-4B49-9EE8-34CDB52550BF}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="G14" sqref="G14:G15"/>
     </sheetView>
   </sheetViews>
@@ -2706,7 +2839,7 @@
     </row>
     <row r="3" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="23" t="s">
         <v>43</v>
       </c>
       <c r="C3" s="7" t="e" vm="1">
@@ -2728,7 +2861,7 @@
     </row>
     <row r="4" spans="1:7" ht="41.85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
-      <c r="B4" s="20"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7">
         <f>Wartości!C8^2*Obliczenia!E3</f>
@@ -2943,7 +3076,7 @@
       <c r="F14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="23" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2964,7 +3097,7 @@
       <c r="F15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="20"/>
+      <c r="G15" s="24"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
@@ -3056,7 +3189,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -3064,7 +3197,7 @@
       </c>
     </row>
     <row r="5" spans="2:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="21"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
@@ -3077,4 +3210,608 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3D168F-8193-48C2-A836-A970089A9B71}">
+  <dimension ref="B3:K23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>0.621</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H14" si="0">F4*G4</f>
+        <v>6.21</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>9.18</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>14.6</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>2.88</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1.42</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9">
+        <v>1.78E-2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.89</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10">
+        <v>2.29E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>1.145</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11">
+        <v>0.11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1.18</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>1.18</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+      <c r="G12">
+        <v>2.7099999999999999E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>2.71</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>1.369</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>6.8449999999999998</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14">
+        <v>360</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="26"/>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1.601</v>
+      </c>
+      <c r="H15">
+        <f>F15*G15</f>
+        <v>1.601</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>2.11</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16:H22" si="1">F16*G16</f>
+        <v>2.11</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="26"/>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>3.33</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="26"/>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1.391</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>1.391</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="26"/>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>2.66</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>2.66</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="K19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="26"/>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>20</v>
+      </c>
+      <c r="G20">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" s="26"/>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>2.0100000000000002</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="26"/>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>2.98</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <f>SUM(H4:H22)</f>
+        <v>70.89200000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I19" r:id="rId1" xr:uid="{9D179B2B-B626-4039-AA10-913C8FAD0832}"/>
+    <hyperlink ref="J19" r:id="rId2" xr:uid="{26F16354-B81D-4BE8-B630-D6513999E7F0}"/>
+    <hyperlink ref="I17" r:id="rId3" xr:uid="{66DAC25C-F7F8-4F97-A074-115EEA2D318D}"/>
+    <hyperlink ref="J17" r:id="rId4" xr:uid="{A522D6C4-322F-4A71-8B03-5EE1BD569785}"/>
+    <hyperlink ref="I18" r:id="rId5" xr:uid="{3109E308-12C9-49B8-8316-305703109B34}"/>
+    <hyperlink ref="J18" r:id="rId6" xr:uid="{5CF39041-3CD7-4C16-B34D-FB9A74FDA35B}"/>
+    <hyperlink ref="I16" r:id="rId7" xr:uid="{443A547F-EE9E-48EB-9ADB-16BD67D0F72B}"/>
+    <hyperlink ref="I15" r:id="rId8" xr:uid="{6CAEB753-E0CC-416D-9B8B-A0D263603741}"/>
+    <hyperlink ref="J15" r:id="rId9" xr:uid="{65CB9033-2BCB-424E-B18F-DD3C40E85CF3}"/>
+    <hyperlink ref="I14" r:id="rId10" xr:uid="{C6DA9541-FB70-4077-B933-1D2F8E27B0E8}"/>
+    <hyperlink ref="I13" r:id="rId11" xr:uid="{E4A951AA-778C-41BF-AFED-71A83F2C0ED2}"/>
+    <hyperlink ref="I12" r:id="rId12" xr:uid="{F17FC927-CB90-4F06-9463-1E4911D99779}"/>
+    <hyperlink ref="I11" r:id="rId13" xr:uid="{ABD7E977-C753-47B9-92CC-ABA785EA32D3}"/>
+    <hyperlink ref="I4" r:id="rId14" xr:uid="{278B6474-1F62-4FB8-881D-9FF02A7D4D5A}"/>
+    <hyperlink ref="I5" r:id="rId15" xr:uid="{B4AFCEC6-5DA7-4582-AD78-D66CCBF86176}"/>
+    <hyperlink ref="I6" r:id="rId16" xr:uid="{724D5967-ABD5-41FC-A7A1-BC1BB7C390B9}"/>
+    <hyperlink ref="I7" r:id="rId17" xr:uid="{D78C49D7-D80E-477D-9A42-323B32F63CB6}"/>
+    <hyperlink ref="I8" r:id="rId18" xr:uid="{ABE4195D-8CEF-4A0D-B2F4-CB686BAF7C2E}"/>
+    <hyperlink ref="I9" r:id="rId19" xr:uid="{4166BAF3-215D-4FBB-9C64-01C3A559DA81}"/>
+    <hyperlink ref="I10" r:id="rId20" xr:uid="{076C426A-2208-426E-81E0-BA021378284D}"/>
+    <hyperlink ref="I22" r:id="rId21" xr:uid="{490C924E-D178-4DA4-9A4B-3E933BDE8659}"/>
+    <hyperlink ref="I20" r:id="rId22" xr:uid="{92260A3C-A8F1-4E2D-90AB-1314F89C7FD9}"/>
+    <hyperlink ref="I21" r:id="rId23" xr:uid="{557E7441-45FF-4F6D-A569-D99FF79231A5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ostatnie poprawki do schematu
</commit_message>
<xml_diff>
--- a/dokumentacja.xlsx
+++ b/dokumentacja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piotr\Documents\mos\laser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241BEA0D-6BEA-49D8-B05A-13988747313B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17EC080-3A41-45BA-ADBB-E19654742E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{C786B773-E517-459C-88A4-5CBE983CE902}"/>
   </bookViews>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="141">
   <si>
     <t>Nazwa</t>
   </si>
@@ -1409,9 +1409,6 @@
     <t>dioda</t>
   </si>
   <si>
-    <t>SS34</t>
-  </si>
-  <si>
     <t>cewka</t>
   </si>
   <si>
@@ -1482,6 +1479,15 @@
   </si>
   <si>
     <t>JST 2 pin</t>
+  </si>
+  <si>
+    <t>B340A</t>
+  </si>
+  <si>
+    <t>bezpiecznik</t>
+  </si>
+  <si>
+    <t>fast 2.5A</t>
   </si>
 </sst>
 </file>
@@ -3214,10 +3220,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3D168F-8193-48C2-A836-A970089A9B71}">
-  <dimension ref="B3:K23"/>
+  <dimension ref="B3:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3242,24 +3248,24 @@
         <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G3" t="s">
         <v>108</v>
       </c>
       <c r="H3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" t="s">
         <v>123</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>124</v>
-      </c>
-      <c r="K3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C4">
         <v>47</v>
@@ -3281,12 +3287,12 @@
         <v>6.21</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C5">
         <v>22</v>
@@ -3308,12 +3314,12 @@
         <v>9.18</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -3335,12 +3341,12 @@
         <v>14.6</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3362,12 +3368,12 @@
         <v>2.88</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3389,7 +3395,7 @@
         <v>1.42</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
@@ -3416,7 +3422,7 @@
         <v>0.89</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
@@ -3443,7 +3449,7 @@
         <v>1.145</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
@@ -3460,17 +3466,17 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G11">
         <v>1.18</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>1.18</v>
+        <v>5.8999999999999995</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
@@ -3497,12 +3503,12 @@
         <v>2.71</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C13">
         <v>20</v>
@@ -3524,7 +3530,7 @@
         <v>6.8449999999999998</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
@@ -3551,7 +3557,7 @@
         <v>1.25</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
@@ -3559,62 +3565,62 @@
         <v>113</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G15">
-        <v>1.601</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="H15">
         <f>F15*G15</f>
-        <v>1.601</v>
+        <v>9.85</v>
       </c>
       <c r="I15" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="J15" s="19" t="s">
         <v>127</v>
-      </c>
-      <c r="J15" s="19" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16">
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G16">
         <v>2.11</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:H22" si="1">F16*G16</f>
-        <v>2.11</v>
+        <f t="shared" ref="H16:H23" si="1">F16*G16</f>
+        <v>6.33</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="26" t="s">
         <v>117</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>118</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17">
@@ -3631,43 +3637,43 @@
         <v>3.33</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="26" t="s">
         <v>119</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>120</v>
       </c>
       <c r="D18" s="26"/>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G18">
-        <v>1.391</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>1.391</v>
+        <v>5.75</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>3</v>
@@ -3677,31 +3683,31 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G19">
         <v>2.66</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>2.66</v>
+        <v>7.98</v>
       </c>
       <c r="I19" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="J19" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="J19" s="19" t="s">
-        <v>127</v>
-      </c>
       <c r="K19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D20" s="26"/>
       <c r="E20">
@@ -3718,15 +3724,15 @@
         <v>6.5</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21">
@@ -3743,15 +3749,15 @@
         <v>2.0100000000000002</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22">
@@ -3768,17 +3774,46 @@
         <v>2.98</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23" s="26"/>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>1.46</v>
+      </c>
       <c r="H23">
-        <f>SUM(H4:H22)</f>
-        <v>70.89200000000001</v>
+        <f t="shared" si="1"/>
+        <v>7.3</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <f>SUM(H4:H23)</f>
+        <v>105.06000000000002</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C15:D15"/>
@@ -3811,6 +3846,8 @@
     <hyperlink ref="I22" r:id="rId21" xr:uid="{490C924E-D178-4DA4-9A4B-3E933BDE8659}"/>
     <hyperlink ref="I20" r:id="rId22" xr:uid="{92260A3C-A8F1-4E2D-90AB-1314F89C7FD9}"/>
     <hyperlink ref="I21" r:id="rId23" xr:uid="{557E7441-45FF-4F6D-A569-D99FF79231A5}"/>
+    <hyperlink ref="I23" r:id="rId24" display="https://www.tme.eu/pl/details/erbrg2r50v/bezpieczniki-smd-1206-szybkie/panasonic/" xr:uid="{8E27A859-9E82-4E54-9DF6-D99CAC4FF851}"/>
+    <hyperlink ref="J23" r:id="rId25" xr:uid="{D9B9EC61-E2C6-4995-A462-46200B92B199}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Teraz już na pewno statnie poprawki do schematu
</commit_message>
<xml_diff>
--- a/dokumentacja.xlsx
+++ b/dokumentacja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piotr\Documents\mos\laser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17EC080-3A41-45BA-ADBB-E19654742E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CACC82-514B-404B-ACF9-540328542954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{C786B773-E517-459C-88A4-5CBE983CE902}"/>
   </bookViews>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="143">
   <si>
     <t>Nazwa</t>
   </si>
@@ -1424,9 +1424,6 @@
     <t>stabilizator</t>
   </si>
   <si>
-    <t>AMS1117</t>
-  </si>
-  <si>
     <t>driver</t>
   </si>
   <si>
@@ -1475,9 +1472,6 @@
     <t>konektor laser</t>
   </si>
   <si>
-    <t>JST 3 pin</t>
-  </si>
-  <si>
     <t>JST 2 pin</t>
   </si>
   <si>
@@ -1488,6 +1482,18 @@
   </si>
   <si>
     <t>fast 2.5A</t>
+  </si>
+  <si>
+    <t>AP2210</t>
+  </si>
+  <si>
+    <t>molex KK 396 3 pin</t>
+  </si>
+  <si>
+    <t>molex KK 396 2 pin</t>
+  </si>
+  <si>
+    <t>zielona</t>
   </si>
 </sst>
 </file>
@@ -3220,10 +3226,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3D168F-8193-48C2-A836-A970089A9B71}">
-  <dimension ref="B3:K24"/>
+  <dimension ref="B3:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3248,24 +3254,24 @@
         <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G3" t="s">
         <v>108</v>
       </c>
       <c r="H3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" t="s">
         <v>122</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>123</v>
-      </c>
-      <c r="K3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4">
         <v>47</v>
@@ -3287,12 +3293,12 @@
         <v>6.21</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C5">
         <v>22</v>
@@ -3314,12 +3320,12 @@
         <v>9.18</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -3341,12 +3347,12 @@
         <v>14.6</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3368,12 +3374,12 @@
         <v>2.88</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3395,7 +3401,7 @@
         <v>1.42</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
@@ -3422,7 +3428,7 @@
         <v>0.89</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
@@ -3449,7 +3455,7 @@
         <v>1.145</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
@@ -3476,7 +3482,7 @@
         <v>5.8999999999999995</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
@@ -3503,12 +3509,12 @@
         <v>2.71</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13">
         <v>20</v>
@@ -3530,7 +3536,7 @@
         <v>6.8449999999999998</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
@@ -3538,7 +3544,7 @@
         <v>111</v>
       </c>
       <c r="C14">
-        <v>360</v>
+        <v>330</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -3550,14 +3556,14 @@
         <v>100</v>
       </c>
       <c r="G14">
-        <v>1.2500000000000001E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>1.25</v>
+        <v>0.4</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
@@ -3565,7 +3571,7 @@
         <v>113</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15">
@@ -3582,10 +3588,10 @@
         <v>9.85</v>
       </c>
       <c r="I15" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="J15" s="19" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
@@ -3608,11 +3614,11 @@
         <v>2.11</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:H23" si="1">F16*G16</f>
+        <f t="shared" ref="H16:H24" si="1">F16*G16</f>
         <v>6.33</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
@@ -3637,10 +3643,10 @@
         <v>3.33</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
@@ -3648,7 +3654,7 @@
         <v>118</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="D18" s="26"/>
       <c r="E18">
@@ -3658,22 +3664,20 @@
         <v>5</v>
       </c>
       <c r="G18">
-        <v>1.1499999999999999</v>
+        <v>0.23</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>5.75</v>
+        <v>1.1500000000000001</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="J18" s="18" t="s">
         <v>126</v>
       </c>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>3</v>
@@ -3693,46 +3697,46 @@
         <v>7.98</v>
       </c>
       <c r="I19" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="J19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="J19" s="19" t="s">
-        <v>126</v>
-      </c>
       <c r="K19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D20" s="26"/>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G20">
-        <v>0.32500000000000001</v>
+        <v>0.71</v>
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
-        <v>6.5</v>
+        <v>7.1</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21">
@@ -3749,15 +3753,15 @@
         <v>2.0100000000000002</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22">
@@ -3767,22 +3771,22 @@
         <v>10</v>
       </c>
       <c r="G22">
-        <v>0.29799999999999999</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="H22">
         <f t="shared" si="1"/>
-        <v>2.98</v>
+        <v>5.6599999999999993</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23">
@@ -3792,27 +3796,53 @@
         <v>5</v>
       </c>
       <c r="G23">
-        <v>1.46</v>
+        <v>0.41</v>
       </c>
       <c r="H23">
         <f t="shared" si="1"/>
-        <v>7.3</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>127</v>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>126</v>
       </c>
       <c r="J23" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="26"/>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>3.39E-2</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>0.33899999999999997</v>
+      </c>
+      <c r="I24" s="19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H24">
-        <f>SUM(H4:H23)</f>
-        <v>105.06000000000002</v>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <f>SUM(H4:H24)</f>
+        <v>97.979000000000013</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
@@ -3828,26 +3858,26 @@
     <hyperlink ref="I17" r:id="rId3" xr:uid="{66DAC25C-F7F8-4F97-A074-115EEA2D318D}"/>
     <hyperlink ref="J17" r:id="rId4" xr:uid="{A522D6C4-322F-4A71-8B03-5EE1BD569785}"/>
     <hyperlink ref="I18" r:id="rId5" xr:uid="{3109E308-12C9-49B8-8316-305703109B34}"/>
-    <hyperlink ref="J18" r:id="rId6" xr:uid="{5CF39041-3CD7-4C16-B34D-FB9A74FDA35B}"/>
-    <hyperlink ref="I16" r:id="rId7" xr:uid="{443A547F-EE9E-48EB-9ADB-16BD67D0F72B}"/>
-    <hyperlink ref="I15" r:id="rId8" xr:uid="{6CAEB753-E0CC-416D-9B8B-A0D263603741}"/>
-    <hyperlink ref="J15" r:id="rId9" xr:uid="{65CB9033-2BCB-424E-B18F-DD3C40E85CF3}"/>
-    <hyperlink ref="I14" r:id="rId10" xr:uid="{C6DA9541-FB70-4077-B933-1D2F8E27B0E8}"/>
-    <hyperlink ref="I13" r:id="rId11" xr:uid="{E4A951AA-778C-41BF-AFED-71A83F2C0ED2}"/>
-    <hyperlink ref="I12" r:id="rId12" xr:uid="{F17FC927-CB90-4F06-9463-1E4911D99779}"/>
-    <hyperlink ref="I11" r:id="rId13" xr:uid="{ABD7E977-C753-47B9-92CC-ABA785EA32D3}"/>
-    <hyperlink ref="I4" r:id="rId14" xr:uid="{278B6474-1F62-4FB8-881D-9FF02A7D4D5A}"/>
-    <hyperlink ref="I5" r:id="rId15" xr:uid="{B4AFCEC6-5DA7-4582-AD78-D66CCBF86176}"/>
-    <hyperlink ref="I6" r:id="rId16" xr:uid="{724D5967-ABD5-41FC-A7A1-BC1BB7C390B9}"/>
-    <hyperlink ref="I7" r:id="rId17" xr:uid="{D78C49D7-D80E-477D-9A42-323B32F63CB6}"/>
-    <hyperlink ref="I8" r:id="rId18" xr:uid="{ABE4195D-8CEF-4A0D-B2F4-CB686BAF7C2E}"/>
-    <hyperlink ref="I9" r:id="rId19" xr:uid="{4166BAF3-215D-4FBB-9C64-01C3A559DA81}"/>
-    <hyperlink ref="I10" r:id="rId20" xr:uid="{076C426A-2208-426E-81E0-BA021378284D}"/>
-    <hyperlink ref="I22" r:id="rId21" xr:uid="{490C924E-D178-4DA4-9A4B-3E933BDE8659}"/>
-    <hyperlink ref="I20" r:id="rId22" xr:uid="{92260A3C-A8F1-4E2D-90AB-1314F89C7FD9}"/>
-    <hyperlink ref="I21" r:id="rId23" xr:uid="{557E7441-45FF-4F6D-A569-D99FF79231A5}"/>
-    <hyperlink ref="I23" r:id="rId24" display="https://www.tme.eu/pl/details/erbrg2r50v/bezpieczniki-smd-1206-szybkie/panasonic/" xr:uid="{8E27A859-9E82-4E54-9DF6-D99CAC4FF851}"/>
-    <hyperlink ref="J23" r:id="rId25" xr:uid="{D9B9EC61-E2C6-4995-A462-46200B92B199}"/>
+    <hyperlink ref="I16" r:id="rId6" xr:uid="{443A547F-EE9E-48EB-9ADB-16BD67D0F72B}"/>
+    <hyperlink ref="I15" r:id="rId7" xr:uid="{6CAEB753-E0CC-416D-9B8B-A0D263603741}"/>
+    <hyperlink ref="J15" r:id="rId8" xr:uid="{65CB9033-2BCB-424E-B18F-DD3C40E85CF3}"/>
+    <hyperlink ref="I14" r:id="rId9" xr:uid="{C6DA9541-FB70-4077-B933-1D2F8E27B0E8}"/>
+    <hyperlink ref="I13" r:id="rId10" xr:uid="{E4A951AA-778C-41BF-AFED-71A83F2C0ED2}"/>
+    <hyperlink ref="I12" r:id="rId11" xr:uid="{F17FC927-CB90-4F06-9463-1E4911D99779}"/>
+    <hyperlink ref="I11" r:id="rId12" xr:uid="{ABD7E977-C753-47B9-92CC-ABA785EA32D3}"/>
+    <hyperlink ref="I4" r:id="rId13" xr:uid="{278B6474-1F62-4FB8-881D-9FF02A7D4D5A}"/>
+    <hyperlink ref="I5" r:id="rId14" xr:uid="{B4AFCEC6-5DA7-4582-AD78-D66CCBF86176}"/>
+    <hyperlink ref="I6" r:id="rId15" xr:uid="{724D5967-ABD5-41FC-A7A1-BC1BB7C390B9}"/>
+    <hyperlink ref="I7" r:id="rId16" xr:uid="{D78C49D7-D80E-477D-9A42-323B32F63CB6}"/>
+    <hyperlink ref="I8" r:id="rId17" xr:uid="{ABE4195D-8CEF-4A0D-B2F4-CB686BAF7C2E}"/>
+    <hyperlink ref="I9" r:id="rId18" xr:uid="{4166BAF3-215D-4FBB-9C64-01C3A559DA81}"/>
+    <hyperlink ref="I10" r:id="rId19" xr:uid="{076C426A-2208-426E-81E0-BA021378284D}"/>
+    <hyperlink ref="I22" r:id="rId20" xr:uid="{490C924E-D178-4DA4-9A4B-3E933BDE8659}"/>
+    <hyperlink ref="I20" r:id="rId21" xr:uid="{92260A3C-A8F1-4E2D-90AB-1314F89C7FD9}"/>
+    <hyperlink ref="I21" r:id="rId22" xr:uid="{557E7441-45FF-4F6D-A569-D99FF79231A5}"/>
+    <hyperlink ref="I23" r:id="rId23" display="https://www.tme.eu/pl/details/erbrg2r50v/bezpieczniki-smd-1206-szybkie/panasonic/" xr:uid="{8E27A859-9E82-4E54-9DF6-D99CAC4FF851}"/>
+    <hyperlink ref="J23" r:id="rId24" xr:uid="{D9B9EC61-E2C6-4995-A462-46200B92B199}"/>
+    <hyperlink ref="I24" r:id="rId25" xr:uid="{EAB7CF42-40BC-4CEE-B470-49728B7564BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>